<commit_message>
Gestion de l'intrface equipier
</commit_message>
<xml_diff>
--- a/documentation/tab_Wacdo_Manager.xlsx
+++ b/documentation/tab_Wacdo_Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/t7/Examen/Wacdo_Manager/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C5BF17-C7A2-A34E-89D3-FC33A96FAF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF15324-82D0-B144-B687-311DCE69C906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{76F3A711-AAFE-6B43-BF03-CC836A88D949}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>Nom controleur</t>
   </si>
@@ -253,7 +253,7 @@
     <t>$listeCategories(objet categories), $listeProduit(objet Products)</t>
   </si>
   <si>
-    <t>$listeUsers</t>
+    <t>$listeUsers(objet utilisateur)</t>
   </si>
 </sst>
 </file>
@@ -751,7 +751,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,7 +799,9 @@
       <c r="C3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
@@ -811,7 +813,9 @@
       <c r="C4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -827,7 +831,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
@@ -837,7 +841,9 @@
       <c r="C6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
@@ -942,8 +948,8 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
mise a jour des doc
</commit_message>
<xml_diff>
--- a/documentation/tab_Wacdo_Manager.xlsx
+++ b/documentation/tab_Wacdo_Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/t7/Examen/Wacdo_Manager/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF15324-82D0-B144-B687-311DCE69C906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B4E9A-2393-7A4A-9099-A58B4D568005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{76F3A711-AAFE-6B43-BF03-CC836A88D949}"/>
+    <workbookView xWindow="51200" yWindow="1440" windowWidth="38400" windowHeight="21600" xr2:uid="{76F3A711-AAFE-6B43-BF03-CC836A88D949}"/>
   </bookViews>
   <sheets>
     <sheet name="view" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Nom controleur</t>
   </si>
@@ -76,12 +76,6 @@
     <t>passer le statut de la commande a livrer</t>
   </si>
   <si>
-    <t>livrer_commande</t>
-  </si>
-  <si>
-    <t>ajouter_produit</t>
-  </si>
-  <si>
     <t>ajouter des produit a la commande en cours</t>
   </si>
   <si>
@@ -91,18 +85,9 @@
     <t>suppression de la commande en cours</t>
   </si>
   <si>
-    <t>supprimer_utilisateur</t>
-  </si>
-  <si>
-    <t>supprime un utilisateur de la base de donnée</t>
-  </si>
-  <si>
     <t>enregistrer les modification des données de l'ulisisateur</t>
   </si>
   <si>
-    <t>afficher_detail_commande</t>
-  </si>
-  <si>
     <t xml:space="preserve">affiche le detail de la commande selectionner </t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>$_GET['id'] de la commande en cours</t>
   </si>
   <si>
-    <t>$_GET['id'] de l'utilisateur. Concerné</t>
-  </si>
-  <si>
     <t>$_POST['nom','prenom',email','statut']</t>
   </si>
   <si>
@@ -254,6 +236,18 @@
   </si>
   <si>
     <t>$listeUsers(objet utilisateur)</t>
+  </si>
+  <si>
+    <t>displayDetailOrder</t>
+  </si>
+  <si>
+    <t>$listOrder(liste insexé par l'id), $detailOrder(liste Indexé par l'id); $orderCurrent(comande selectionné)</t>
+  </si>
+  <si>
+    <t>addOrderDetail</t>
+  </si>
+  <si>
+    <t>delivreryOrder</t>
   </si>
 </sst>
 </file>
@@ -750,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D4333D-8F63-744A-9CF7-F695D83E2049}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -763,7 +757,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -777,72 +771,72 @@
     </row>
     <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.2">
@@ -948,8 +942,8 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,7 +969,7 @@
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -984,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -998,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.2">
@@ -1012,231 +1006,237 @@
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" x14ac:dyDescent="0.2">

</xml_diff>